<commit_message>
Subida de busqueda de camino
</commit_message>
<xml_diff>
--- a/mediciones.xlsx
+++ b/mediciones.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d7f3f8e23c5cac0d/Documentos/CAM_Windows/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1919" documentId="13_ncr:1_{018A9B68-6C3D-4EE8-8E1E-431342C0410A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3D6BA838-3DE7-4FD0-9CB7-1BEA27E96F42}"/>
+  <xr:revisionPtr revIDLastSave="1956" documentId="13_ncr:1_{018A9B68-6C3D-4EE8-8E1E-431342C0410A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FD463C81-CEDE-4DBF-817B-796B1A282032}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="824" firstSheet="5" activeTab="6" xr2:uid="{D5AAE986-D25D-4ED4-8DFE-8E0C7A09621E}"/>
+    <workbookView xWindow="75" yWindow="1260" windowWidth="16065" windowHeight="11385" tabRatio="824" firstSheet="6" activeTab="13" xr2:uid="{D5AAE986-D25D-4ED4-8DFE-8E0C7A09621E}"/>
   </bookViews>
   <sheets>
-    <sheet name="CAM Basica" sheetId="21" r:id="rId1"/>
+    <sheet name="CAM Simple" sheetId="21" r:id="rId1"/>
     <sheet name="CAM Simple Optimizada" sheetId="6" r:id="rId2"/>
     <sheet name="CAM Simple-Opt-Con parada" sheetId="7" r:id="rId3"/>
     <sheet name="CAM Binaria" sheetId="8" r:id="rId4"/>
@@ -1465,7 +1465,85 @@
           </a:r>
           <a:r>
             <a:rPr lang="es-ES" sz="1100" baseline="0"/>
-            <a:t> único defecto de este modelo de CAM es que necesitas dos memorias del tamaño de N para almacenar los índices de cada nodo, y que cada vez que se actualice el árbol habrá que actualizar los índices también. </a:t>
+            <a:t> único defecto de este modelo de CAM es que necesitas memoria adicional para los indices, cuyo tamaño es N para almacenar los índices de cada nodo, y que cada vez que se actualice el árbol habrá que actualizar los índices también. </a:t>
+          </a:r>
+          <a:endParaRPr lang="es-ES" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="CuadroTexto 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20A959B6-6144-4A91-B914-F03E86860954}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7943850" y="2733675"/>
+          <a:ext cx="4667250" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent5">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100"/>
+            <a:t>No merece la pena dar dos hijos por ciclo</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+            <a:t> porque no vamos a tener que consumir mas de dos hijos por ciclo</a:t>
           </a:r>
           <a:endParaRPr lang="es-ES" sz="1100"/>
         </a:p>
@@ -3360,7 +3438,7 @@
   <dimension ref="A1:T184"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4602,7 +4680,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5367,8 +5445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E48CE571-B250-4D9B-A485-A8953DCBB074}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5411,13 +5489,13 @@
         <v>31</v>
       </c>
       <c r="D2">
+        <v>32</v>
+      </c>
+      <c r="E2">
         <v>31</v>
       </c>
-      <c r="E2">
-        <v>33</v>
-      </c>
       <c r="F2">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G2">
         <v>40</v>
@@ -5431,22 +5509,22 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="C3">
         <v>71</v>
       </c>
       <c r="D3">
+        <v>76</v>
+      </c>
+      <c r="E3">
         <v>78</v>
       </c>
-      <c r="E3">
-        <v>79</v>
-      </c>
       <c r="F3">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G3">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H3">
         <v>102</v>
@@ -5457,22 +5535,22 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C4">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D4">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E4">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F4">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="G4">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="H4">
         <v>56</v>
@@ -5509,25 +5587,25 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G6">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="H6">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -5561,22 +5639,22 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>6.7629999999999999</v>
+        <v>6.6230000000000002</v>
       </c>
       <c r="C8">
-        <v>7.343</v>
+        <v>7.2430000000000003</v>
       </c>
       <c r="D8">
-        <v>7.1189999999999998</v>
+        <v>7.86</v>
       </c>
       <c r="E8">
-        <v>7.2350000000000003</v>
+        <v>7.5350000000000001</v>
       </c>
       <c r="F8">
-        <v>7.52</v>
+        <v>7.6109999999999998</v>
       </c>
       <c r="G8">
-        <v>7.7080000000000002</v>
+        <v>8.6029999999999998</v>
       </c>
       <c r="H8">
         <v>7.8789999999999996</v>
@@ -5740,7 +5818,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5749,7 +5828,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8085,8 +8164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB42CDD6-E79B-46D8-999D-4F0F638D6E86}">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8868,7 +8947,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Avances en operaciones Scone
</commit_message>
<xml_diff>
--- a/mediciones.xlsx
+++ b/mediciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d7f3f8e23c5cac0d/Documentos/CAM_Windows/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1956" documentId="13_ncr:1_{018A9B68-6C3D-4EE8-8E1E-431342C0410A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FD463C81-CEDE-4DBF-817B-796B1A282032}"/>
+  <xr:revisionPtr revIDLastSave="1974" documentId="13_ncr:1_{018A9B68-6C3D-4EE8-8E1E-431342C0410A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ED045732-406C-44EE-B2BA-851BDB680044}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="1260" windowWidth="16065" windowHeight="11385" tabRatio="824" firstSheet="6" activeTab="13" xr2:uid="{D5AAE986-D25D-4ED4-8DFE-8E0C7A09621E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="824" firstSheet="6" activeTab="13" xr2:uid="{D5AAE986-D25D-4ED4-8DFE-8E0C7A09621E}"/>
   </bookViews>
   <sheets>
     <sheet name="CAM Simple" sheetId="21" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="14">
   <si>
     <t>Como podemos comprobar, no hay prácticamente cambios en utilizar la estrategia de usar el almacenamiento de los datos del árbol tanto en anchura como en profundidad. El coste de recursos crece lógicamente con el crecimiento del árbol, siendo lo más destacable el requerimiento de usar 15 BRAMs para guardar los datos del árbol. El uso tanto de FFs como de LUTs crece también pero de manera muy poco significativa. Vemos que la latencia sigue el orden de O(2N) siendo N el tamaño del árbol.</t>
   </si>
@@ -95,7 +95,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,8 +132,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,6 +161,11 @@
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
       </patternFill>
     </fill>
   </fills>
@@ -181,14 +193,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -202,10 +215,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="60% - Énfasis5" xfId="4" builtinId="48"/>
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Énfasis2" xfId="5" builtinId="33"/>
     <cellStyle name="Entrada" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Texto explicativo" xfId="2" builtinId="53"/>
@@ -1279,15 +1294,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>236376</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>103987</xdr:rowOff>
+      <xdr:colOff>341151</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>189712</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1310,7 +1325,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9525" y="3114675"/>
+          <a:off x="114300" y="4914900"/>
           <a:ext cx="7322976" cy="4799812"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1475,16 +1490,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1499,7 +1514,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7943850" y="2733675"/>
+          <a:off x="7248525" y="2466975"/>
           <a:ext cx="4667250" cy="628650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5443,10 +5458,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E48CE571-B250-4D9B-A485-A8953DCBB074}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5814,6 +5829,72 @@
       </c>
       <c r="H15">
         <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18">
+        <v>643</v>
+      </c>
+      <c r="H18">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19">
+        <v>42563</v>
+      </c>
+      <c r="H19">
+        <v>87333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20">
+        <v>6</v>
+      </c>
+      <c r="H20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21">
+        <v>645</v>
+      </c>
+      <c r="H21">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22">
+        <v>42565</v>
+      </c>
+      <c r="H22">
+        <v>87344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>